<commit_message>
Add cement CC lci
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-carbon-capture.xlsx
+++ b/premise/data/additional_inventories/lci-carbon-capture.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D415D5-20A1-8348-8410-7999E2D72DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6F1CAA-B366-124C-987A-6B2C9F87ED9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31960" yWindow="60" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DAC!$A$1:$T$366</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DAC!$A$1:$T$361</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="265">
   <si>
     <t>Activity</t>
   </si>
@@ -744,6 +744,96 @@
   </si>
   <si>
     <t>operation. Uncertainty from deJong et al., 2021</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured at cement production plant, using monoethanolamine</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured at cement plant</t>
+  </si>
+  <si>
+    <t>Carbon capture using MEA: Main source: Voldsund (2019) - CEMCAP - D4.6 CEMCAP comparative techno-economic analysis. Heat for MEA regeneration now produced with same fuel mix as MEA kiln (not natural gas as in Voldsund). Transport and storage from Premise inventories. 90% CO2 capture efficiency (process+fuel CO2). Source: Amelie Müller, Carina Harpprecht, Romain Sacchi, Ben Maes, Mariësse van Sluisveld, Vassilis Daioglou, Branko Šavija, Bernhard Steubing, Decarbonizing the cement industry: Findings from coupling prospective life cycle assessment of clinker with integrated assessment model scenarios, Journal of Cleaner Production, 2024, https://doi.org/10.1016/j.jclepro.2024.141884.</t>
+  </si>
+  <si>
+    <t>MEA mark-up, lost in reclaimer (1.4 kg MEA/tCO2) CEMCAP - D4.6 CEMCAP comparative techno-economic analysis, p. 26</t>
+  </si>
+  <si>
+    <t>Electricity consumption for fans, pumps and thermal reclaimer (188 MJ/tclk [primary energy], 761 kg CO2/tclk, 0.459 conversion factor primary to secondary energy, 3.6 MJ/kWh) CEMCAP - D4.6 CEMCAP comparative techno-economic analysis, Table 5.3</t>
+  </si>
+  <si>
+    <t>Electricity consumption for cooling water system (123 MJ/tclk [primary energy], 761 kg CO2/tclk, 0.459 conversion factor primary to secondary energy, 3.6 MJ/kWh) CEMCAP - D4.6 CEMCAP comparative techno-economic analysis, Table 5.3</t>
+  </si>
+  <si>
+    <t>market group for tap water</t>
+  </si>
+  <si>
+    <t>Process water mark-up. CEMCAP - D4.6 CEMCAP comparative techno-economic analysis, Table 5.1</t>
+  </si>
+  <si>
+    <t>Spent MEA solvent: Share of airborne emission and solid emissions from Moser 2011</t>
+  </si>
+  <si>
+    <t>Monoethanolamine</t>
+  </si>
+  <si>
+    <t>MEA emissions, rest is regenerated. Share of airborne emission and solid emissions (process: treatment of spent solvent mixture) from Moser 2011</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Steam for MEA regeneration (3.76 MJ/kg CO2, of which 0.11 can be recuberated from waste heat).</t>
+  </si>
+  <si>
+    <t>steam production, as energy carrier, in chemical industry</t>
+  </si>
+  <si>
+    <t>carbon dioxide storage from hard coal, post, pipeline 200km, storage 1000m</t>
+  </si>
+  <si>
+    <t>Amelie Müller, Carina Harpprecht, Romain Sacchi, Ben Maes, Mariësse van Sluisveld, Vassilis Daioglou, Branko Šavija, Bernhard Steubing, Decarbonizing the cement industry: Findings from coupling prospective life cycle assessment of clinker with integrated assessment model scenarios, Journal of Cleaner Production, 2024, https://doi.org/10.1016/j.jclepro.2024.141884.</t>
+  </si>
+  <si>
+    <t>Energy needed for compression and liquefication of CO2 (CPU): (CEMCAP D4.6, table 5.3)</t>
+  </si>
+  <si>
+    <t>SOx removal, needed so that MEA doesn't form amine salts. Stochiometric amount of 1.25 kg NaOH/kg SOx is sufficient (Cempcap 4.6). 0.00035 kg SOx/kg clinker (ecoinvent), 0.828 kg CO2/kg clinker from GCCA data.</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured at cement production plant, using direct separation</t>
+  </si>
+  <si>
+    <t>Carbon capture using Direct Separation. Main source: LEILAC project https://ec.europa.eu/research/participants/documents/downloadPublic?documentIds=080166e5df29e8fc&amp;appId=PPGMS. 95% capture efficiency of process related emissions.  Source: Amelie Müller, Carina Harpprecht, Romain Sacchi, Ben Maes, Mariësse van Sluisveld, Vassilis Daioglou, Branko Šavija, Bernhard Steubing, Decarbonizing the cement industry: Findings from coupling prospective life cycle assessment of clinker with integrated assessment model scenarios, Journal of Cleaner Production, 2024, https://doi.org/10.1016/j.jclepro.2024.141884.</t>
+  </si>
+  <si>
+    <t>Additional electricity for LEILAC: LEILAC D3.6 Life Cycle Assessment, Table 4-6: 77kWh/t clinker, Table 4-1: 0.558 t process emissions/t clinker</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured at cement production plant, using oxyfuel</t>
+  </si>
+  <si>
+    <t>Carbon capture with Oxyfuel technology, where fuel combustion happens in Oxygen-CO2-mix instead of air, which creates a cleaner CO2 flue gas stream. Main source: Voldsund (2019) - CEMCAP - D4.6 CEMCAP comparative techno-economic analysis. 90% CO2 capture efficiency (process+fuel CO2). Includes changes in electricity demand due to new kiln design for oxy-process, oxygen production with ASU, CO2 compression and purification, CO2 transport. Excludes changes in Non-CO2 emissions: CPU reduces SOx (99.99%), NOx (99.36%), Hg (100%) and CO (100%). Source: Amelie Müller, Carina Harpprecht, Romain Sacchi, Ben Maes, Mariësse van Sluisveld, Vassilis Daioglou, Branko Šavija, Bernhard Steubing, Decarbonizing the cement industry: Findings from coupling prospective life cycle assessment of clinker with integrated assessment model scenarios, Journal of Cleaner Production, 2024, https://doi.org/10.1016/j.jclepro.2024.141884.</t>
+  </si>
+  <si>
+    <t>stochiometric amount of O2 needed for combustion with pure oxygen. 11% losses due flue gas looping are already included in the ASU process</t>
+  </si>
+  <si>
+    <t>Electricity savings due to equipment changes: additional fans +122 MJ/tclk , electric power generation -182 MJ/tclk with organic rankine cycle, energy savings at Fans, milling, and handling of solids in kiln -62 MJ/tclk, [all in primary energy], 758 kg CO2/tclk, Conversion factor primary to secondary energy 0.459, 3.6 MJ/kWh. Voldsund (2019) - CEMCAP - D4.6 CEMCAP comparative techno-economic analysis, Table 6.3</t>
+  </si>
+  <si>
+    <t>Electricity consumption cooling water system. 59 MJ/tclk [primary energy], 758 kg CO2/tclk, Conversion factor primary to secondary energy 0.459, 3.6 MJ/kWh. Voldsund (2019) - CEMCAP - D4.6 CEMCAP comparative techno-economic analysis, Table 6.3</t>
+  </si>
+  <si>
+    <t>Compression and purification: Electricity for CPU (440 KJ/kgCO2) (CEMCAP D4.6, table 6.1)</t>
+  </si>
+  <si>
+    <t>industrial gases production, cryogenic air separation</t>
+  </si>
+  <si>
+    <t>oxygen, liquid</t>
+  </si>
+  <si>
+    <t>Compression and purification unit: Electricity for cooling system (0.03 KJ/kg CO2) (CEMCAP D4.6, table 6.1)</t>
   </si>
 </sst>
 </file>
@@ -757,9 +847,9 @@
     <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="174" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="169" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -841,6 +931,22 @@
       <sz val="12"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -863,7 +969,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -889,10 +995,16 @@
     <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1208,19 +1320,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T366"/>
+  <dimension ref="A1:T380"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="C377" sqref="C377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="79.5" customWidth="1"/>
+    <col min="1" max="1" width="47.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -1518,7 +1630,7 @@
       <c r="A19" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="24">
         <f>-1*B17</f>
         <v>-4.0000000000000001E-3</v>
       </c>
@@ -1542,7 +1654,7 @@
       <c r="A20" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="25">
         <f>-1*B18</f>
         <v>-3.5000000000000001E-3</v>
       </c>
@@ -1932,7 +2044,7 @@
       <c r="A41" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="25">
+      <c r="B41" s="24">
         <f>-1*B39</f>
         <v>-4.0000000000000001E-3</v>
       </c>
@@ -1956,7 +2068,7 @@
       <c r="A42" t="s">
         <v>75</v>
       </c>
-      <c r="B42" s="26">
+      <c r="B42" s="25">
         <f>-1*B40</f>
         <v>-3.5000000000000001E-3</v>
       </c>
@@ -3114,7 +3226,7 @@
       <c r="I111">
         <v>5</v>
       </c>
-      <c r="J111" s="24">
+      <c r="J111" s="23">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="K111">
@@ -3352,7 +3464,7 @@
       <c r="A125" t="s">
         <v>19</v>
       </c>
-      <c r="B125" s="23" t="s">
+      <c r="B125" t="s">
         <v>231</v>
       </c>
     </row>
@@ -3705,7 +3817,7 @@
       <c r="A144" t="s">
         <v>19</v>
       </c>
-      <c r="B144" s="23" t="s">
+      <c r="B144" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4346,7 +4458,7 @@
       <c r="A179" t="s">
         <v>19</v>
       </c>
-      <c r="B179" s="23" t="s">
+      <c r="B179" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4875,7 +4987,7 @@
         <v>93</v>
       </c>
       <c r="B217">
-        <f>AVERAGE(K217:L217)</f>
+        <f t="shared" ref="B217:B227" si="0">AVERAGE(K217:L217)</f>
         <v>1.9749999999999999</v>
       </c>
       <c r="C217" t="s">
@@ -4909,7 +5021,7 @@
         <v>85</v>
       </c>
       <c r="B218">
-        <f>AVERAGE(K218:L218)</f>
+        <f t="shared" si="0"/>
         <v>3.1749999999999998</v>
       </c>
       <c r="C218" t="s">
@@ -4928,7 +5040,7 @@
         <v>5</v>
       </c>
       <c r="J218">
-        <f t="shared" ref="J218:J227" si="0">B218</f>
+        <f t="shared" ref="J218:J227" si="1">B218</f>
         <v>3.1749999999999998</v>
       </c>
       <c r="K218">
@@ -4943,7 +5055,7 @@
         <v>94</v>
       </c>
       <c r="B219">
-        <f>AVERAGE(K219:L219)</f>
+        <f t="shared" si="0"/>
         <v>2.59</v>
       </c>
       <c r="C219" t="s">
@@ -4962,7 +5074,7 @@
         <v>5</v>
       </c>
       <c r="J219">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.59</v>
       </c>
       <c r="K219">
@@ -4977,7 +5089,7 @@
         <v>95</v>
       </c>
       <c r="B220">
-        <f>AVERAGE(K220:L220)</f>
+        <f t="shared" si="0"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="C220" t="s">
@@ -4996,7 +5108,7 @@
         <v>5</v>
       </c>
       <c r="J220">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="K220">
@@ -5011,7 +5123,7 @@
         <v>94</v>
       </c>
       <c r="B221">
-        <f>AVERAGE(K221:L221)</f>
+        <f t="shared" si="0"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="C221" t="s">
@@ -5030,7 +5142,7 @@
         <v>5</v>
       </c>
       <c r="J221">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="K221">
@@ -5045,7 +5157,7 @@
         <v>96</v>
       </c>
       <c r="B222">
-        <f>AVERAGE(K222:L222)</f>
+        <f t="shared" si="0"/>
         <v>0.11570000000000008</v>
       </c>
       <c r="C222" t="s">
@@ -5067,7 +5179,7 @@
         <v>5</v>
       </c>
       <c r="J222">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11570000000000008</v>
       </c>
       <c r="K222">
@@ -5084,7 +5196,7 @@
         <v>97</v>
       </c>
       <c r="B223">
-        <f>AVERAGE(K223:L223)</f>
+        <f t="shared" si="0"/>
         <v>1.3817000000000013</v>
       </c>
       <c r="C223" t="s">
@@ -5106,7 +5218,7 @@
         <v>5</v>
       </c>
       <c r="J223">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3817000000000013</v>
       </c>
       <c r="K223">
@@ -5123,7 +5235,7 @@
         <v>87</v>
       </c>
       <c r="B224">
-        <f>AVERAGE(K224:L224)</f>
+        <f t="shared" si="0"/>
         <v>14.559999999999999</v>
       </c>
       <c r="C224" t="s">
@@ -5142,7 +5254,7 @@
         <v>5</v>
       </c>
       <c r="J224">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.559999999999999</v>
       </c>
       <c r="K224">
@@ -5157,7 +5269,7 @@
         <v>35</v>
       </c>
       <c r="B225">
-        <f>AVERAGE(K225:L225)</f>
+        <f t="shared" si="0"/>
         <v>0.34499999999999997</v>
       </c>
       <c r="C225" t="s">
@@ -5176,7 +5288,7 @@
         <v>5</v>
       </c>
       <c r="J225">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.34499999999999997</v>
       </c>
       <c r="K225">
@@ -5191,7 +5303,7 @@
         <v>86</v>
       </c>
       <c r="B226">
-        <f>AVERAGE(K226:L226)</f>
+        <f t="shared" si="0"/>
         <v>7.4749999999999996</v>
       </c>
       <c r="C226" t="s">
@@ -5210,7 +5322,7 @@
         <v>5</v>
       </c>
       <c r="J226">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4749999999999996</v>
       </c>
       <c r="K226">
@@ -5225,7 +5337,7 @@
         <v>74</v>
       </c>
       <c r="B227">
-        <f>AVERAGE(K227:L227)</f>
+        <f t="shared" si="0"/>
         <v>-1.5</v>
       </c>
       <c r="C227" t="s">
@@ -5244,7 +5356,7 @@
         <v>5</v>
       </c>
       <c r="J227">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.5</v>
       </c>
       <c r="K227">
@@ -7181,7 +7293,7 @@
         <v>0.16679850853156178</v>
       </c>
     </row>
-    <row r="321" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>32</v>
       </c>
@@ -7231,7 +7343,7 @@
         <v>0.16679850853156178</v>
       </c>
     </row>
-    <row r="322" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>35</v>
       </c>
@@ -7281,7 +7393,7 @@
         <v>0.16679850853156178</v>
       </c>
     </row>
-    <row r="323" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>195</v>
       </c>
@@ -7332,7 +7444,7 @@
         <v>0.16679850853156178</v>
       </c>
     </row>
-    <row r="324" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A324" s="21" t="s">
         <v>93</v>
       </c>
@@ -7382,36 +7494,845 @@
         <v>0.16679850853156178</v>
       </c>
     </row>
-    <row r="330" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A330" s="1"/>
-      <c r="B330" s="1"/>
-    </row>
-    <row r="337" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A337" s="1"/>
-    </row>
-    <row r="344" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A344" s="1"/>
-      <c r="B344" s="1"/>
-    </row>
-    <row r="346" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B346" s="2"/>
-    </row>
-    <row r="351" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A351" s="1"/>
-    </row>
-    <row r="353" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A353" s="2"/>
-      <c r="J353" s="2"/>
-    </row>
-    <row r="359" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A359" s="1"/>
-      <c r="B359" s="1"/>
-    </row>
-    <row r="366" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A366" s="1"/>
+    <row r="326" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A326" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B326" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="327" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A327" t="s">
+        <v>7</v>
+      </c>
+      <c r="B327" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="328" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A328" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B328">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A329" t="s">
+        <v>2</v>
+      </c>
+      <c r="B329" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="330" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A330" t="s">
+        <v>3</v>
+      </c>
+      <c r="B330" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="331" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A331" t="s">
+        <v>5</v>
+      </c>
+      <c r="B331" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="332" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A332" t="s">
+        <v>19</v>
+      </c>
+      <c r="B332" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="333" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A333" t="s">
+        <v>9</v>
+      </c>
+      <c r="B333" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="334" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A334" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="335" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A335" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C335" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D335" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E335" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F335" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G335" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H335" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I335" s="5"/>
+      <c r="J335" s="5"/>
+      <c r="K335" s="5"/>
+      <c r="L335" s="5"/>
+      <c r="M335" s="5"/>
+      <c r="N335" s="5"/>
+      <c r="O335" s="5"/>
+      <c r="P335" s="5"/>
+      <c r="Q335" s="5"/>
+      <c r="R335" s="5"/>
+      <c r="S335" s="5"/>
+    </row>
+    <row r="336" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A336" s="28" t="str">
+        <f>B326</f>
+        <v>carbon dioxide, captured at cement production plant, using monoethanolamine</v>
+      </c>
+      <c r="B336" s="28">
+        <v>1</v>
+      </c>
+      <c r="C336" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D336" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F336" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G336" s="28" t="str">
+        <f>B329</f>
+        <v>carbon dioxide, captured at cement plant</v>
+      </c>
+    </row>
+    <row r="337" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A337" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B337" s="29">
+        <v>1</v>
+      </c>
+      <c r="C337" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D337" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F337" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G337" s="28" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="338" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A338" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B338" s="29">
+        <f>1.4/1000</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="C338" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D338" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F338" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G338" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="H338" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="N338" s="29"/>
+    </row>
+    <row r="339" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A339" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B339" s="29">
+        <f>0.000355*1.25*(1/0.828)</f>
+        <v>5.3592995169082129E-4</v>
+      </c>
+      <c r="C339" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D339" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F339" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G339" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="H339" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="N339" s="29"/>
+      <c r="P339" s="29"/>
+    </row>
+    <row r="340" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A340" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="B340" s="29">
+        <f>(3.76-0.11)/0.9</f>
+        <v>4.0555555555555554</v>
+      </c>
+      <c r="C340" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D340" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F340" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G340" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="H340" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="N340" s="29"/>
+    </row>
+    <row r="341" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A341" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B341" s="29">
+        <f>188/761*0.459/3.6</f>
+        <v>3.1498028909329831E-2</v>
+      </c>
+      <c r="C341" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D341" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F341" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G341" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H341" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="N341" s="29"/>
+    </row>
+    <row r="342" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A342" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B342" s="29">
+        <f>123/761*0.459/3.6</f>
+        <v>2.0607752956636003E-2</v>
+      </c>
+      <c r="C342" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D342" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F342" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G342" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H342" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="N342" s="29"/>
+    </row>
+    <row r="343" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A343" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B343" s="29">
+        <f>575/761*0.459/3.6</f>
+        <v>9.63370565045992E-2</v>
+      </c>
+      <c r="C343" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D343" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F343" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G343" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H343" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="N343" s="29"/>
+      <c r="Q343" s="30"/>
+    </row>
+    <row r="344" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A344" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="B344" s="29">
+        <f>0.473</f>
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="C344" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D344" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F344" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G344" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="H344" s="28" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="345" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A345" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B345" s="29">
+        <f>-B338*0.227/(0.227+0.006)</f>
+        <v>-1.3639484978540772E-3</v>
+      </c>
+      <c r="C345" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D345" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F345" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G345" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="H345" s="28" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="346" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A346" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B346" s="29">
+        <f>1.4/1000*(0.006/0.227+0.006)</f>
+        <v>4.5404405286343617E-5</v>
+      </c>
+      <c r="D346" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E346" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F346" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H346" s="28" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="347" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A347" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B347" s="29">
+        <f>B344/1000</f>
+        <v>4.7299999999999995E-4</v>
+      </c>
+      <c r="D347" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="E347" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F347" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G347" s="29"/>
+    </row>
+    <row r="349" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A349" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B349" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="350" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A350" t="s">
+        <v>7</v>
+      </c>
+      <c r="B350" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="351" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A351" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B351">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A352" t="s">
+        <v>2</v>
+      </c>
+      <c r="B352" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="353" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A353" t="s">
+        <v>3</v>
+      </c>
+      <c r="B353" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="354" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A354" t="s">
+        <v>5</v>
+      </c>
+      <c r="B354" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="355" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A355" t="s">
+        <v>19</v>
+      </c>
+      <c r="B355" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="356" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A356" t="s">
+        <v>9</v>
+      </c>
+      <c r="B356" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="357" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A357" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="358" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A358" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C358" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D358" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E358" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F358" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G358" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H358" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I358" s="5"/>
+      <c r="J358" s="5"/>
+      <c r="K358" s="5"/>
+      <c r="L358" s="5"/>
+      <c r="M358" s="5"/>
+      <c r="N358" s="5"/>
+      <c r="O358" s="5"/>
+      <c r="P358" s="5"/>
+      <c r="Q358" s="5"/>
+      <c r="R358" s="5"/>
+      <c r="S358" s="5"/>
+    </row>
+    <row r="359" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A359" s="28" t="str">
+        <f>B349</f>
+        <v>carbon dioxide, captured at cement production plant, using direct separation</v>
+      </c>
+      <c r="B359" s="28">
+        <v>1</v>
+      </c>
+      <c r="C359" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D359" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F359" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G359" s="28" t="str">
+        <f>B352</f>
+        <v>carbon dioxide, captured at cement plant</v>
+      </c>
+    </row>
+    <row r="360" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A360" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B360" s="29">
+        <v>1</v>
+      </c>
+      <c r="C360" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D360" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E360" s="28"/>
+      <c r="F360" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G360" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="H360" s="28"/>
+    </row>
+    <row r="361" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A361" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B361" s="32">
+        <f>77*1/0.558/1000</f>
+        <v>0.13799283154121864</v>
+      </c>
+      <c r="C361" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D361" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F361" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G361" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H361" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="N361" s="32"/>
+    </row>
+    <row r="364" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A364" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B364" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="365" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A365" t="s">
+        <v>7</v>
+      </c>
+      <c r="B365" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="366" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A366" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B366">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A367" t="s">
+        <v>2</v>
+      </c>
+      <c r="B367" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="368" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A368" t="s">
+        <v>3</v>
+      </c>
+      <c r="B368" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="369" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A369" t="s">
+        <v>5</v>
+      </c>
+      <c r="B369" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="370" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A370" t="s">
+        <v>19</v>
+      </c>
+      <c r="B370" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="371" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A371" t="s">
+        <v>9</v>
+      </c>
+      <c r="B371" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="372" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A372" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="373" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A373" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C373" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D373" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E373" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F373" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G373" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H373" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I373" s="5"/>
+      <c r="J373" s="5"/>
+      <c r="K373" s="5"/>
+      <c r="L373" s="5"/>
+      <c r="M373" s="5"/>
+      <c r="N373" s="5"/>
+      <c r="O373" s="5"/>
+      <c r="P373" s="5"/>
+      <c r="Q373" s="5"/>
+      <c r="R373" s="5"/>
+      <c r="S373" s="5"/>
+    </row>
+    <row r="374" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A374" s="28" t="str">
+        <f>B364</f>
+        <v>carbon dioxide, captured at cement production plant, using oxyfuel</v>
+      </c>
+      <c r="B374" s="28">
+        <v>1</v>
+      </c>
+      <c r="C374" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D374" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F374" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G374" s="28" t="str">
+        <f>B367</f>
+        <v>carbon dioxide, captured at cement plant</v>
+      </c>
+    </row>
+    <row r="375" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A375" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B375" s="29">
+        <v>1</v>
+      </c>
+      <c r="C375" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D375" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E375" s="28"/>
+      <c r="F375" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G375" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="H375" s="28"/>
+    </row>
+    <row r="376" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A376" t="s">
+        <v>262</v>
+      </c>
+      <c r="B376" s="6">
+        <f>B374*32/44/(1-0.11)</f>
+        <v>0.81716036772216549</v>
+      </c>
+      <c r="C376" t="s">
+        <v>27</v>
+      </c>
+      <c r="D376" t="s">
+        <v>6</v>
+      </c>
+      <c r="F376" t="s">
+        <v>16</v>
+      </c>
+      <c r="G376" t="s">
+        <v>263</v>
+      </c>
+      <c r="H376" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="377" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A377" t="s">
+        <v>35</v>
+      </c>
+      <c r="B377" s="6">
+        <f>(122-182-62)/758*0.459/3.6</f>
+        <v>-2.0521108179419524E-2</v>
+      </c>
+      <c r="C377" t="s">
+        <v>8</v>
+      </c>
+      <c r="D377" t="s">
+        <v>24</v>
+      </c>
+      <c r="F377" t="s">
+        <v>16</v>
+      </c>
+      <c r="G377" t="s">
+        <v>25</v>
+      </c>
+      <c r="H377" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="378" spans="1:19" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A378" t="s">
+        <v>35</v>
+      </c>
+      <c r="B378" s="6">
+        <f>59/758*0.459/3.6</f>
+        <v>9.9241424802110813E-3</v>
+      </c>
+      <c r="C378" t="s">
+        <v>8</v>
+      </c>
+      <c r="D378" t="s">
+        <v>24</v>
+      </c>
+      <c r="F378" t="s">
+        <v>16</v>
+      </c>
+      <c r="G378" t="s">
+        <v>25</v>
+      </c>
+      <c r="H378" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="379" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A379" t="s">
+        <v>35</v>
+      </c>
+      <c r="B379" s="6">
+        <f>440/3600</f>
+        <v>0.12222222222222222</v>
+      </c>
+      <c r="C379" t="s">
+        <v>8</v>
+      </c>
+      <c r="D379" t="s">
+        <v>24</v>
+      </c>
+      <c r="F379" t="s">
+        <v>16</v>
+      </c>
+      <c r="G379" t="s">
+        <v>25</v>
+      </c>
+      <c r="H379" t="s">
+        <v>261</v>
+      </c>
+      <c r="M379" s="27"/>
+      <c r="N379" s="31"/>
+    </row>
+    <row r="380" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A380" t="s">
+        <v>35</v>
+      </c>
+      <c r="B380" s="6">
+        <f>0.03/3600</f>
+        <v>8.3333333333333337E-6</v>
+      </c>
+      <c r="C380" t="s">
+        <v>8</v>
+      </c>
+      <c r="D380" t="s">
+        <v>24</v>
+      </c>
+      <c r="F380" t="s">
+        <v>16</v>
+      </c>
+      <c r="G380" t="s">
+        <v>25</v>
+      </c>
+      <c r="H380" t="s">
+        <v>264</v>
+      </c>
+      <c r="M380" s="27"/>
+      <c r="N380" s="31"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T366" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:T361" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove "World" from default value in "except regions"
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-carbon-capture.xlsx
+++ b/premise/data/additional_inventories/lci-carbon-capture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080B30BA-B161-3B46-B804-43A28BD59505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846C32FD-FF81-8E44-A374-EC8B073AB5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="264">
   <si>
     <t>Activity</t>
   </si>
@@ -780,9 +780,6 @@
   </si>
   <si>
     <t>Water</t>
-  </si>
-  <si>
-    <t>steam production, as energy carrier, in chemical industry</t>
   </si>
   <si>
     <t>carbon dioxide storage from hard coal, post, pipeline 200km, storage 1000m</t>
@@ -1323,7 +1320,7 @@
   <dimension ref="A1:T380"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
-      <selection activeCell="H341" sqref="H341"/>
+      <selection activeCell="C341" sqref="C341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7547,7 +7544,7 @@
         <v>19</v>
       </c>
       <c r="B332" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="333" spans="1:19" x14ac:dyDescent="0.2">
@@ -7624,7 +7621,7 @@
     </row>
     <row r="337" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A337" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B337" s="29">
         <v>1</v>
@@ -7639,7 +7636,7 @@
         <v>16</v>
       </c>
       <c r="G337" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="338" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
@@ -7688,21 +7685,21 @@
         <v>146</v>
       </c>
       <c r="H339" s="28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N339" s="29"/>
       <c r="P339" s="29"/>
     </row>
     <row r="340" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A340" s="28" t="s">
-        <v>247</v>
+        <v>81</v>
       </c>
       <c r="B340" s="29">
         <f>3.76-0.11</f>
         <v>3.65</v>
       </c>
       <c r="C340" s="28" t="s">
-        <v>8</v>
+        <v>135</v>
       </c>
       <c r="D340" s="28" t="s">
         <v>23</v>
@@ -7711,10 +7708,10 @@
         <v>16</v>
       </c>
       <c r="G340" s="28" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="H340" s="28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N340" s="29"/>
     </row>
@@ -7789,7 +7786,7 @@
         <v>25</v>
       </c>
       <c r="H343" s="28" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N343" s="29"/>
       <c r="Q343" s="30"/>
@@ -7887,7 +7884,7 @@
         <v>0</v>
       </c>
       <c r="B349" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="350" spans="1:17" x14ac:dyDescent="0.2">
@@ -7935,7 +7932,7 @@
         <v>19</v>
       </c>
       <c r="B355" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="356" spans="1:19" x14ac:dyDescent="0.2">
@@ -7943,7 +7940,7 @@
         <v>9</v>
       </c>
       <c r="B356" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="357" spans="1:19" x14ac:dyDescent="0.2">
@@ -8012,7 +8009,7 @@
     </row>
     <row r="360" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A360" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B360" s="29">
         <v>1</v>
@@ -8028,7 +8025,7 @@
         <v>16</v>
       </c>
       <c r="G360" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H360" s="28"/>
     </row>
@@ -8053,7 +8050,7 @@
         <v>25</v>
       </c>
       <c r="H361" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N361" s="32"/>
     </row>
@@ -8062,7 +8059,7 @@
         <v>0</v>
       </c>
       <c r="B364" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="365" spans="1:19" x14ac:dyDescent="0.2">
@@ -8110,7 +8107,7 @@
         <v>19</v>
       </c>
       <c r="B370" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="371" spans="1:19" x14ac:dyDescent="0.2">
@@ -8118,7 +8115,7 @@
         <v>9</v>
       </c>
       <c r="B371" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="372" spans="1:19" x14ac:dyDescent="0.2">
@@ -8187,7 +8184,7 @@
     </row>
     <row r="375" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A375" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B375" s="29">
         <v>1</v>
@@ -8203,13 +8200,13 @@
         <v>16</v>
       </c>
       <c r="G375" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H375" s="28"/>
     </row>
     <row r="376" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B376" s="6">
         <f>B374*32/44/(1-0.11)</f>
@@ -8225,10 +8222,10 @@
         <v>16</v>
       </c>
       <c r="G376" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H376" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="377" spans="1:19" x14ac:dyDescent="0.2">
@@ -8252,7 +8249,7 @@
         <v>25</v>
       </c>
       <c r="H377" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="378" spans="1:19" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8276,7 +8273,7 @@
         <v>25</v>
       </c>
       <c r="H378" s="26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="379" spans="1:19" x14ac:dyDescent="0.2">
@@ -8300,7 +8297,7 @@
         <v>25</v>
       </c>
       <c r="H379" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M379" s="27"/>
       <c r="N379" s="31"/>
@@ -8326,7 +8323,7 @@
         <v>25</v>
       </c>
       <c r="H380" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M380" s="27"/>
       <c r="N380" s="31"/>

</xml_diff>

<commit_message>
Add cement CCS datasets
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-carbon-capture.xlsx
+++ b/premise/data/additional_inventories/lci-carbon-capture.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBD57E1-8C1E-404D-AAB1-028A6C86991D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4250949B-9023-E24C-A5C7-1864AA2E9D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -838,13 +838,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="0.0E+00"/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -964,13 +964,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -980,27 +980,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1319,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
-      <selection activeCell="G341" sqref="G341"/>
+    <sheetView tabSelected="1" topLeftCell="A351" workbookViewId="0">
+      <selection activeCell="B377" sqref="B377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>